<commit_message>
Updating readTteb.R to accomodate data update. New script to read microcystin. Stripped microcystin from script for reading algal pigments.
</commit_message>
<xml_diff>
--- a/SuRGE_Sharepoint/data/chemistry/tteb/tteb_prelim_anions_ic.xlsx
+++ b/SuRGE_Sharepoint/data/chemistry/tteb/tteb_prelim_anions_ic.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa.sharepoint.com/sites/SuRGE/Shared Documents/data/chemistry/tteb/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/beaulieu_jake_epa_gov/Documents/gitRepository/SuRGE/SuRGE_Sharepoint/data/chemistry/tteb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{222F4100-3F50-4983-B8C8-E95467080159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFBDA3A4-6057-433B-B2B1-6C59E8F9BCCD}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{222F4100-3F50-4983-B8C8-E95467080159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B3EC1B5-5A56-4052-ACB4-14E3AA2968E7}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{4690DFDB-484E-44B8-ADFB-B917F52F5631}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="74">
   <si>
     <t>lab_id</t>
   </si>
@@ -258,18 +258,6 @@
   </si>
   <si>
     <t>224719 Spk</t>
-  </si>
-  <si>
-    <t>222232</t>
-  </si>
-  <si>
-    <t>222233</t>
-  </si>
-  <si>
-    <t>222234</t>
-  </si>
-  <si>
-    <t>222235</t>
   </si>
 </sst>
 </file>
@@ -329,9 +317,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -369,7 +357,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -475,7 +463,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -617,7 +605,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -625,11 +613,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D364504-65C9-4452-A0B7-27D1440BBDF2}">
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J58" sqref="J58"/>
+      <selection pane="bottomLeft" activeCell="A62" sqref="A62:XFD65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2040,98 +2028,6 @@
         <v>2.9632999999999998</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>74</v>
-      </c>
-      <c r="B62">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C62">
-        <v>13.175599999999999</v>
-      </c>
-      <c r="E62">
-        <v>3.9800000000000002E-2</v>
-      </c>
-      <c r="F62" t="s">
-        <v>11</v>
-      </c>
-      <c r="G62" t="s">
-        <v>12</v>
-      </c>
-      <c r="H62">
-        <v>1.5213000000000001</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>75</v>
-      </c>
-      <c r="B63">
-        <v>2.53E-2</v>
-      </c>
-      <c r="C63">
-        <v>13.222200000000001</v>
-      </c>
-      <c r="E63" t="s">
-        <v>10</v>
-      </c>
-      <c r="F63" t="s">
-        <v>11</v>
-      </c>
-      <c r="G63" t="s">
-        <v>12</v>
-      </c>
-      <c r="H63">
-        <v>1.448</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>76</v>
-      </c>
-      <c r="B64">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C64">
-        <v>13.1294</v>
-      </c>
-      <c r="E64">
-        <v>4.2099999999999999E-2</v>
-      </c>
-      <c r="F64" t="s">
-        <v>11</v>
-      </c>
-      <c r="G64" t="s">
-        <v>12</v>
-      </c>
-      <c r="H64">
-        <v>1.4135</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>77</v>
-      </c>
-      <c r="B65" t="s">
-        <v>8</v>
-      </c>
-      <c r="C65">
-        <v>4.5600000000000002E-2</v>
-      </c>
-      <c r="E65" t="s">
-        <v>10</v>
-      </c>
-      <c r="F65" t="s">
-        <v>11</v>
-      </c>
-      <c r="G65" t="s">
-        <v>12</v>
-      </c>
-      <c r="H65" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2139,20 +2035,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001AF5FC5DD832BE4DBA6B24560DD3ADC0" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d40b3e6283001fb57e5088f84fb23d5e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="8b03727f-4454-4722-b3e6-018d8dcaf2fd" xmlns:ns6="ed970698-2d60-4bab-a048-d9be527522d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="aadbb8160917885bdc8cfb32badaafe9" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2623,6 +2505,20 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2666,9 +2562,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05249EBC-F609-4DFD-B48C-156CB9C347AA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EFE5CC1-E0AC-4A51-9C22-5FA754B99B7A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="8b03727f-4454-4722-b3e6-018d8dcaf2fd"/>
+    <ds:schemaRef ds:uri="ed970698-2d60-4bab-a048-d9be527522d9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2682,9 +2593,23 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EFE5CC1-E0AC-4A51-9C22-5FA754B99B7A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05249EBC-F609-4DFD-B48C-156CB9C347AA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2771CD8D-4A58-45DD-A0C4-BBF11B8B5AED}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2771CD8D-4A58-45DD-A0C4-BBF11B8B5AED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="ed970698-2d60-4bab-a048-d9be527522d9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>